<commit_message>
Author has been Added
</commit_message>
<xml_diff>
--- a/bin/TestData/Data.xlsx
+++ b/bin/TestData/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="ObjectR" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Locator_Type</t>
   </si>
@@ -111,13 +111,25 @@
   </si>
   <si>
     <t>Apple_comp3</t>
+  </si>
+  <si>
+    <t>//input[@title='Search']</t>
+  </si>
+  <si>
+    <t>text_search</t>
+  </si>
+  <si>
+    <t>btn_search</t>
+  </si>
+  <si>
+    <t>//div[@class='FPdoLc VlcLAe']//input[@value='Google Search']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +149,14 @@
       <sz val="10"/>
       <color rgb="FF303336"/>
       <name val="Inherit"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -166,7 +186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -175,6 +195,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -480,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -633,6 +654,28 @@
         <v>26</v>
       </c>
     </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -643,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>